<commit_message>
Test Results for v1.5 - New test cases have been added as TC011
</commit_message>
<xml_diff>
--- a/GroupProject/diagramPDF/testCaseSpreadsheet.xlsx
+++ b/GroupProject/diagramPDF/testCaseSpreadsheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oh it's only you\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oh it's only you\Desktop\cs370\370Fall17Team6\GroupProject\diagramPDF\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="101">
   <si>
     <t>TCID</t>
   </si>
@@ -119,9 +119,6 @@
     <t>"Cancel" closes prompt</t>
   </si>
   <si>
-    <t>Accepts empty string as a valid list name</t>
-  </si>
-  <si>
     <t>List saves changes made to its name on UI</t>
   </si>
   <si>
@@ -164,15 +161,6 @@
     <t>Opens up keyboard prompt for user input</t>
   </si>
   <si>
-    <t>Opens keyboard but deletes previous list</t>
-  </si>
-  <si>
-    <t>Accepts input but deletes list whilst renaming</t>
-  </si>
-  <si>
-    <t>Recreates new empty list instead of renaming</t>
-  </si>
-  <si>
     <t>After tapping, prompts for user confirmation</t>
   </si>
   <si>
@@ -227,9 +215,6 @@
     <t>Search Method</t>
   </si>
   <si>
-    <t>Forces input to be all lowercase before searching DB</t>
-  </si>
-  <si>
     <t>Checks for valid input (no numbers or special chars)</t>
   </si>
   <si>
@@ -290,9 +275,6 @@
     <t>List saves on Item Menu UI when adding items</t>
   </si>
   <si>
-    <t>List does not persist when exiting app</t>
-  </si>
-  <si>
     <t>Item does not persist when exiting to main menu</t>
   </si>
   <si>
@@ -302,9 +284,6 @@
     <t>Checkmark is not a persisting attribute</t>
   </si>
   <si>
-    <t>Name is changed - name does not persist however</t>
-  </si>
-  <si>
     <t>Keyboard takes input and invokes search</t>
   </si>
   <si>
@@ -321,13 +300,43 @@
   </si>
   <si>
     <t>Quantity does not persist</t>
+  </si>
+  <si>
+    <t>TC011</t>
+  </si>
+  <si>
+    <t>TC012</t>
+  </si>
+  <si>
+    <t>Group Type (GBT)</t>
+  </si>
+  <si>
+    <t>Adding an item groups it by type in alphabetical order</t>
+  </si>
+  <si>
+    <t>Grouped Items persist after exiting</t>
+  </si>
+  <si>
+    <t>Empty String is accepted</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>CRASHES ON APOSTROPHE; OTHERWISE WORKS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Forces input to be all lowercase for simple DB search</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -392,6 +401,24 @@
       <family val="1"/>
       <charset val="2"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Wingdings 2"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -446,7 +473,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -508,6 +535,19 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -794,11 +834,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -833,7 +873,7 @@
         <v>2</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="H1" s="21" t="s">
         <v>22</v>
@@ -910,57 +950,59 @@
         <v>20</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>30</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="41">
         <v>4</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="8"/>
+      <c r="E5" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="H5" s="40" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="43">
         <v>5</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>87</v>
+      <c r="E6" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="42" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -992,49 +1034,49 @@
         <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="5">
         <v>1</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="9"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="9" t="s">
+      <c r="C9" s="45">
+        <v>2</v>
+      </c>
+      <c r="D9" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="10">
-        <v>2</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>87</v>
+      <c r="E9" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1042,13 +1084,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="5">
         <v>3</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>17</v>
@@ -1066,13 +1108,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="10">
         <v>4</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>17</v>
@@ -1084,7 +1126,7 @@
         <v>20</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -1092,13 +1134,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" s="26">
         <v>5</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E12" s="27" t="s">
         <v>17</v>
@@ -1116,13 +1158,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="10">
         <v>6</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>17</v>
@@ -1134,7 +1176,7 @@
         <v>20</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1142,13 +1184,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" s="5">
         <v>7</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>17</v>
@@ -1166,13 +1208,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="10">
         <v>8</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>17</v>
@@ -1184,7 +1226,7 @@
         <v>20</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1192,13 +1234,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C16" s="4">
         <v>1</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>17</v>
@@ -1216,13 +1258,13 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" s="4">
         <v>2</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>17</v>
@@ -1240,127 +1282,127 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" s="4">
         <v>3</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="8"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="36">
+        <v>1</v>
+      </c>
+      <c r="D19" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="H18" s="8"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
+      <c r="E19" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B20" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="18">
-        <v>1</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
+      <c r="C20" s="36">
+        <v>2</v>
+      </c>
+      <c r="D20" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B21" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="18">
-        <v>2</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H20" s="9" t="s">
+      <c r="C21" s="36">
+        <v>3</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="36">
+        <v>4</v>
+      </c>
+      <c r="D22" s="35" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="18">
-        <v>3</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="18">
-        <v>4</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>20</v>
+      <c r="E22" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" s="38" t="s">
+        <v>18</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1374,7 +1416,7 @@
         <v>1</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E23" s="13" t="s">
         <v>19</v>
@@ -1386,7 +1428,7 @@
         <v>20</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1400,7 +1442,7 @@
         <v>2</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>17</v>
@@ -1424,7 +1466,7 @@
         <v>3</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E25" s="31" t="s">
         <v>17</v>
@@ -1442,13 +1484,13 @@
         <v>13</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C26" s="15">
         <v>1</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E26" s="16" t="s">
         <v>17</v>
@@ -1466,13 +1508,13 @@
         <v>13</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C27" s="15">
         <v>2</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E27" s="16" t="s">
         <v>17</v>
@@ -1490,13 +1532,13 @@
         <v>13</v>
       </c>
       <c r="B28" s="32" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C28" s="33">
         <v>3</v>
       </c>
       <c r="D28" s="32" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="E28" s="34" t="s">
         <v>17</v>
@@ -1520,7 +1562,7 @@
         <v>2</v>
       </c>
       <c r="D29" s="32" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E29" s="34" t="s">
         <v>17</v>
@@ -1544,7 +1586,7 @@
         <v>3</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E30" s="16" t="s">
         <v>17</v>
@@ -1568,7 +1610,7 @@
         <v>4</v>
       </c>
       <c r="D31" s="32" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E31" s="34" t="s">
         <v>17</v>
@@ -1592,7 +1634,7 @@
         <v>5</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E32" s="19" t="s">
         <v>17</v>
@@ -1604,77 +1646,77 @@
         <v>20</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="35" t="s">
+      <c r="A33" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="35" t="s">
+      <c r="B33" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="36">
+      <c r="C33" s="33">
         <v>6</v>
       </c>
-      <c r="D33" s="35" t="s">
-        <v>60</v>
-      </c>
-      <c r="E33" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="F33" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="G33" s="38" t="s">
+      <c r="D33" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="E33" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" s="25" t="s">
         <v>18</v>
       </c>
       <c r="H33" s="17"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="35" t="s">
+      <c r="A34" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="35" t="s">
+      <c r="B34" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="36">
+      <c r="C34" s="33">
         <v>7</v>
       </c>
-      <c r="D34" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="E34" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="F34" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="G34" s="38" t="s">
+      <c r="D34" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="E34" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="G34" s="25" t="s">
         <v>18</v>
       </c>
       <c r="H34" s="17"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="35" t="s">
+      <c r="A35" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B35" s="35" t="s">
+      <c r="B35" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="36">
+      <c r="C35" s="33">
         <v>8</v>
       </c>
-      <c r="D35" s="35" t="s">
-        <v>62</v>
-      </c>
-      <c r="E35" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="F35" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="G35" s="38" t="s">
+      <c r="D35" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E35" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="G35" s="25" t="s">
         <v>18</v>
       </c>
       <c r="H35" s="17"/>
@@ -1684,13 +1726,13 @@
         <v>14</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C36" s="12">
         <v>1</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E36" s="13" t="s">
         <v>19</v>
@@ -1702,7 +1744,7 @@
         <v>20</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -1710,13 +1752,13 @@
         <v>14</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C37" s="12">
         <v>2</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E37" s="13" t="s">
         <v>19</v>
@@ -1728,7 +1770,7 @@
         <v>20</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -1736,13 +1778,13 @@
         <v>14</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C38" s="12">
         <v>3</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="E38" s="13" t="s">
         <v>19</v>
@@ -1754,7 +1796,7 @@
         <v>20</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:8" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -1762,13 +1804,13 @@
         <v>14</v>
       </c>
       <c r="B39" s="29" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C39" s="30">
         <v>4</v>
       </c>
       <c r="D39" s="29" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E39" s="31" t="s">
         <v>17</v>
@@ -1792,7 +1834,7 @@
         <v>1</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E40" s="16" t="s">
         <v>17</v>
@@ -1816,7 +1858,7 @@
         <v>2</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E41" s="16" t="s">
         <v>17</v>
@@ -1840,7 +1882,7 @@
         <v>3</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E42" s="11" t="s">
         <v>19</v>
@@ -1852,7 +1894,7 @@
         <v>20</v>
       </c>
       <c r="H42" s="17" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -1866,7 +1908,7 @@
         <v>4</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E43" s="16" t="s">
         <v>17</v>
@@ -1881,16 +1923,16 @@
     </row>
     <row r="44" spans="1:8" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B44" s="29" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C44" s="30">
         <v>1</v>
       </c>
       <c r="D44" s="29" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E44" s="31" t="s">
         <v>17</v>
@@ -1905,16 +1947,16 @@
     </row>
     <row r="45" spans="1:8" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B45" s="29" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C45" s="30">
         <v>2</v>
       </c>
       <c r="D45" s="29" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E45" s="31" t="s">
         <v>17</v>
@@ -1929,16 +1971,16 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C46" s="12">
         <v>3</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E46" s="13" t="s">
         <v>19</v>
@@ -1950,21 +1992,21 @@
         <v>20</v>
       </c>
       <c r="H46" s="8" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C47" s="12">
         <v>4</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E47" s="13" t="s">
         <v>17</v>
@@ -1976,21 +2018,21 @@
         <v>20</v>
       </c>
       <c r="H47" s="8" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B48" s="17" t="s">
         <v>75</v>
-      </c>
-      <c r="B48" s="17" t="s">
-        <v>80</v>
       </c>
       <c r="C48" s="18">
         <v>1</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E48" s="11" t="s">
         <v>19</v>
@@ -2002,21 +2044,21 @@
         <v>20</v>
       </c>
       <c r="H48" s="17" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B49" s="17" t="s">
         <v>75</v>
-      </c>
-      <c r="B49" s="17" t="s">
-        <v>80</v>
       </c>
       <c r="C49" s="18">
         <v>2</v>
       </c>
       <c r="D49" s="17" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E49" s="11" t="s">
         <v>19</v>
@@ -2028,21 +2070,21 @@
         <v>20</v>
       </c>
       <c r="H49" s="17" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B50" s="17" t="s">
         <v>75</v>
-      </c>
-      <c r="B50" s="17" t="s">
-        <v>80</v>
       </c>
       <c r="C50" s="18">
         <v>3</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E50" s="11" t="s">
         <v>19</v>
@@ -2054,21 +2096,21 @@
         <v>20</v>
       </c>
       <c r="H50" s="17" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B51" s="17" t="s">
         <v>75</v>
-      </c>
-      <c r="B51" s="17" t="s">
-        <v>80</v>
       </c>
       <c r="C51" s="18">
         <v>4</v>
       </c>
       <c r="D51" s="17" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E51" s="11" t="s">
         <v>19</v>
@@ -2080,7 +2122,59 @@
         <v>20</v>
       </c>
       <c r="H51" s="17" t="s">
-        <v>53</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C52" s="12">
+        <v>1</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E52" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F52" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G52" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H52" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C53" s="12">
+        <v>2</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E53" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F53" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G53" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H53" s="8" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test Cases and Results updated to release v1.6
</commit_message>
<xml_diff>
--- a/GroupProject/diagramPDF/testCaseSpreadsheet.xlsx
+++ b/GroupProject/diagramPDF/testCaseSpreadsheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="107">
   <si>
     <t>TCID</t>
   </si>
@@ -275,9 +275,6 @@
     <t>List saves on Item Menu UI when adding items</t>
   </si>
   <si>
-    <t>Item does not persist when exiting to main menu</t>
-  </si>
-  <si>
     <t>Quantity is not a persisting attribute</t>
   </si>
   <si>
@@ -320,16 +317,37 @@
     <t>Empty String is accepted</t>
   </si>
   <si>
-    <t>FAIL</t>
-  </si>
-  <si>
-    <t>CRASHES ON APOSTROPHE; OTHERWISE WORKS</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Forces input to be all lowercase for simple DB search</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Deletes old list's contents after rename</t>
+  </si>
+  <si>
+    <t>Delete causes many types of issues in DB</t>
+  </si>
+  <si>
+    <t>TC013</t>
+  </si>
+  <si>
+    <t>Suggestions</t>
+  </si>
+  <si>
+    <t>As user types, suggestions appear with search</t>
+  </si>
+  <si>
+    <t>Suggestions reflect available items in the DB</t>
+  </si>
+  <si>
+    <t>Hierarchy Search</t>
+  </si>
+  <si>
+    <t>User can select items available in DB while searching</t>
+  </si>
+  <si>
+    <t>Available items in DB are shown to the user in search</t>
   </si>
 </sst>
 </file>
@@ -473,7 +491,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -533,13 +551,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -548,6 +560,14 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -834,11 +854,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -950,59 +970,59 @@
         <v>20</v>
       </c>
       <c r="H4" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="39">
+        <v>4</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="38" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="40" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B6" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="41">
-        <v>4</v>
-      </c>
-      <c r="D5" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="40" t="s">
-        <v>97</v>
-      </c>
-      <c r="H5" s="40" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="43">
+      <c r="C6" s="30">
         <v>5</v>
       </c>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="44" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="44" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="42" t="s">
-        <v>99</v>
+      <c r="E6" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="38" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1054,29 +1074,29 @@
       <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="45">
+      <c r="C9" s="26">
         <v>2</v>
       </c>
-      <c r="D9" s="38" t="s">
+      <c r="D9" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="35" t="s">
+      <c r="E9" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="32" t="s">
         <v>18</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1104,29 +1124,29 @@
       <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="41">
         <v>4</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>82</v>
+      <c r="E11" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="37" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -1176,7 +1196,7 @@
         <v>20</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1226,7 +1246,7 @@
         <v>20</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1302,107 +1322,107 @@
       <c r="H18" s="8"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="35" t="s">
+      <c r="B19" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="36">
+      <c r="C19" s="33">
         <v>1</v>
       </c>
-      <c r="D19" s="35" t="s">
+      <c r="D19" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>99</v>
+      <c r="E19" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="25" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="36">
+      <c r="C20" s="33">
         <v>2</v>
       </c>
-      <c r="D20" s="35" t="s">
+      <c r="D20" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="G20" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>99</v>
+      <c r="E20" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" s="25" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="35" t="s">
+      <c r="B21" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="36">
+      <c r="C21" s="44">
         <v>3</v>
       </c>
-      <c r="D21" s="35" t="s">
+      <c r="D21" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="E21" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>99</v>
+      <c r="E21" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="42" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="36">
+      <c r="C22" s="33">
         <v>4</v>
       </c>
-      <c r="D22" s="35" t="s">
+      <c r="D22" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="E22" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="F22" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="G22" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>99</v>
+      <c r="E22" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22" s="25" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1538,7 +1558,7 @@
         <v>3</v>
       </c>
       <c r="D28" s="32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E28" s="34" t="s">
         <v>17</v>
@@ -1646,7 +1666,7 @@
         <v>20</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1744,7 +1764,7 @@
         <v>20</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -1784,7 +1804,7 @@
         <v>3</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E38" s="13" t="s">
         <v>19</v>
@@ -1894,7 +1914,7 @@
         <v>20</v>
       </c>
       <c r="H42" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -1992,7 +2012,7 @@
         <v>20</v>
       </c>
       <c r="H46" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -2018,85 +2038,85 @@
         <v>20</v>
       </c>
       <c r="H47" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="17" t="s">
+      <c r="A48" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="B48" s="17" t="s">
+      <c r="B48" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="C48" s="18">
+      <c r="C48" s="36">
         <v>1</v>
       </c>
-      <c r="D48" s="17" t="s">
+      <c r="D48" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="E48" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F48" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G48" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H48" s="17" t="s">
-        <v>49</v>
+      <c r="E48" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="F48" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="G48" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="H48" s="35" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="17" t="s">
+      <c r="A49" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="B49" s="17" t="s">
+      <c r="B49" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="C49" s="18">
+      <c r="C49" s="36">
         <v>2</v>
       </c>
-      <c r="D49" s="17" t="s">
+      <c r="D49" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="E49" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F49" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G49" s="9" t="s">
-        <v>20</v>
+      <c r="E49" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="F49" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="G49" s="37" t="s">
+        <v>18</v>
       </c>
       <c r="H49" s="17" t="s">
-        <v>49</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="17" t="s">
+      <c r="A50" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="B50" s="17" t="s">
+      <c r="B50" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="C50" s="18">
+      <c r="C50" s="36">
         <v>3</v>
       </c>
-      <c r="D50" s="17" t="s">
+      <c r="D50" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="E50" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F50" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G50" s="9" t="s">
-        <v>20</v>
+      <c r="E50" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="F50" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="G50" s="37" t="s">
+        <v>18</v>
       </c>
       <c r="H50" s="17" t="s">
-        <v>49</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -2122,21 +2142,21 @@
         <v>20</v>
       </c>
       <c r="H51" s="17" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C52" s="12">
         <v>1</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E52" s="13" t="s">
         <v>19</v>
@@ -2153,16 +2173,16 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B53" s="8" t="s">
         <v>92</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>93</v>
       </c>
       <c r="C53" s="12">
         <v>2</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E53" s="13" t="s">
         <v>19</v>
@@ -2174,6 +2194,110 @@
         <v>20</v>
       </c>
       <c r="H53" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B54" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C54" s="18">
+        <v>1</v>
+      </c>
+      <c r="D54" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="E54" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F54" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G54" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H54" s="17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B55" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C55" s="18">
+        <v>2</v>
+      </c>
+      <c r="D55" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="E55" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F55" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G55" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H55" s="17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C56" s="12">
+        <v>1</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E56" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F56" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G56" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H56" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C57" s="12">
+        <v>2</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E57" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F57" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G57" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H57" s="8" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>